<commit_message>
device ip change handeling implementation
</commit_message>
<xml_diff>
--- a/src/devices/edge_devices_v0.0.1.xlsx
+++ b/src/devices/edge_devices_v0.0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044bsj\Desktop\API_app_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C814D157-CFF9-4BBB-A97E-23AD83F472F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72EE89B-2941-45D2-AC92-F812D4E09692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24495" yWindow="0" windowWidth="19590" windowHeight="12360" activeTab="1" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
   </bookViews>
   <sheets>
     <sheet name="DEVICE_CONFIG" sheetId="7" r:id="rId1"/>
@@ -179,7 +179,7 @@
     <t>00:0C:29:FC:EA:3E, 00:0C:29:FC:EA:48</t>
   </si>
   <si>
-    <t>192.168.1.91, 192.168.1.109</t>
+    <t>192.168.1.108, 192.168.1.109</t>
   </si>
 </sst>
 </file>
@@ -621,8 +621,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
index.js handeling request when device IP is different
</commit_message>
<xml_diff>
--- a/src/devices/edge_devices_v0.0.1.xlsx
+++ b/src/devices/edge_devices_v0.0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044bsj\Desktop\API_app_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72EE89B-2941-45D2-AC92-F812D4E09692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20ABB4E-EB2B-45E8-84B7-FC83EDACB4A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
   </bookViews>
@@ -179,7 +179,7 @@
     <t>00:0C:29:FC:EA:3E, 00:0C:29:FC:EA:48</t>
   </si>
   <si>
-    <t>192.168.1.108, 192.168.1.109</t>
+    <t>192.168.1.92, 192.168.1.109</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>